<commit_message>
fix failing tests: output file name now depends on the dates
</commit_message>
<xml_diff>
--- a/tests/data/name_typo/expected/kozep_proba_osszegzes_input.xlsx
+++ b/tests/data/name_typo/expected/kozep_proba_osszegzes_input.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Email</t>
   </si>
@@ -25,6 +25,15 @@
   </si>
   <si>
     <t>Össz.</t>
+  </si>
+  <si>
+    <t>2025.12.01</t>
+  </si>
+  <si>
+    <t>2025.12.08</t>
+  </si>
+  <si>
+    <t>2025.12.15</t>
   </si>
   <si>
     <t>gipszjakab@gmail.com</t>
@@ -55,9 +64,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
-  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11.000000"/>
@@ -108,12 +114,9 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf fontId="1" fillId="0" borderId="1" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -659,74 +662,74 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2">
-        <v>45992</v>
-      </c>
-      <c r="E1" s="2">
-        <v>45999</v>
-      </c>
-      <c r="F1" s="2">
-        <v>46006</v>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -738,7 +741,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{002C0053-00E5-4173-9EC7-0064006C0081}">
+          <x14:cfRule type="expression" priority="1" id="{0076009B-0076-45A1-AAA7-00E0003B00F2}">
             <xm:f>MOD(ROW(),2)=0</xm:f>
             <x14:dxf>
               <fill>
@@ -754,7 +757,7 @@
                 </right>
                 <top style="none"/>
                 <bottom style="none"/>
-                <diagonal/>
+                <diagonal style="none"/>
                 <vertical style="none"/>
                 <horizontal style="none"/>
               </border>
@@ -763,7 +766,7 @@
           <xm:sqref>A2:F4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="2" id="{000400D1-00A3-4082-A127-00BE00DE00E4}">
+          <x14:cfRule type="expression" priority="2" id="{00DA00B0-00DC-4C14-8725-0055007B0073}">
             <xm:f>MOD(ROW(),2)=1</xm:f>
             <x14:dxf>
               <fill>
@@ -779,7 +782,7 @@
                 </right>
                 <top style="none"/>
                 <bottom style="none"/>
-                <diagonal/>
+                <diagonal style="none"/>
                 <vertical style="none"/>
                 <horizontal style="none"/>
               </border>

</xml_diff>